<commit_message>
Update lists of functions
</commit_message>
<xml_diff>
--- a/all_functions.xlsx
+++ b/all_functions.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmuschelli/Dropbox/Teaching/intro_to_r/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avahoffman/Dropbox/JHSPH/intro_to_r/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B73779-53A8-F748-9D97-95BC7A46E59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -119,15 +120,9 @@
     <t>str_extract</t>
   </si>
   <si>
-    <t>gather</t>
-  </si>
-  <si>
     <t>take columns and turn them into observations</t>
   </si>
   <si>
-    <t>spread</t>
-  </si>
-  <si>
     <t>take observations and turn them into columns</t>
   </si>
   <si>
@@ -741,12 +736,18 @@
   </si>
   <si>
     <t>package</t>
+  </si>
+  <si>
+    <t>pivot_longer</t>
+  </si>
+  <si>
+    <t>pivot_wider</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -840,6 +841,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1107,11 +1111,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D113" sqref="A1:D113"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1136,16 +1140,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1156,7 +1160,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -1164,100 +1168,100 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1265,7 +1269,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -1276,27 +1280,27 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -1304,27 +1308,27 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -1332,16 +1336,16 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1349,7 +1353,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1360,27 +1364,27 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
@@ -1391,7 +1395,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
@@ -1405,7 +1409,7 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
@@ -1419,7 +1423,7 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -1433,7 +1437,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
@@ -1447,7 +1451,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
@@ -1461,7 +1465,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
@@ -1475,7 +1479,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C26" t="s">
         <v>26</v>
@@ -1489,7 +1493,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -1503,10 +1507,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
@@ -1514,13 +1518,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>236</v>
+      </c>
+      <c r="B29" t="s">
+        <v>196</v>
+      </c>
+      <c r="C29" t="s">
         <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>198</v>
-      </c>
-      <c r="C29" t="s">
-        <v>31</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
@@ -1528,13 +1532,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>237</v>
       </c>
       <c r="B30" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
@@ -1542,13 +1546,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
@@ -1556,13 +1560,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
@@ -1570,13 +1574,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
         <v>8</v>
@@ -1584,13 +1588,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -1598,13 +1602,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
@@ -1612,44 +1616,44 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1657,7 +1661,7 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
@@ -1671,7 +1675,7 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C40" t="s">
         <v>10</v>
@@ -1682,155 +1686,155 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" t="s">
         <v>62</v>
-      </c>
-      <c r="D45" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D48" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D49" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B51" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C51" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D51" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D52" t="s">
         <v>8</v>
@@ -1838,13 +1842,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D53" t="s">
         <v>8</v>
@@ -1852,13 +1856,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C54" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D54" t="s">
         <v>8</v>
@@ -1866,55 +1870,55 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C55" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D55" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C56" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D56" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B57" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D58" t="s">
         <v>8</v>
@@ -1922,55 +1926,55 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B59" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C59" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B60" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C60" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D60" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C61" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B62" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D62" t="s">
         <v>8</v>
@@ -1978,13 +1982,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B63" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C63" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D63" t="s">
         <v>8</v>
@@ -1992,13 +1996,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B64" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C64" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D64" t="s">
         <v>8</v>
@@ -2006,41 +2010,41 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C66" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B67" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C67" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D67" t="s">
         <v>8</v>
@@ -2048,83 +2052,83 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B68" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C68" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D68" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B69" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C69" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D69" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B70" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C70" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D70" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B71" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C71" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D71" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B72" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C72" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D72" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B73" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C73" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D73" t="s">
         <v>8</v>
@@ -2132,13 +2136,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B74" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C74" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D74" t="s">
         <v>8</v>
@@ -2146,13 +2150,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B75" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C75" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D75" t="s">
         <v>8</v>
@@ -2160,13 +2164,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B76" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C76" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D76" t="s">
         <v>8</v>
@@ -2174,13 +2178,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B77" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C77" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D77" t="s">
         <v>8</v>
@@ -2188,13 +2192,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C78" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D78" t="s">
         <v>8</v>
@@ -2202,41 +2206,41 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B79" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C79" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D79" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B80" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C80" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D80" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B81" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D81" t="s">
         <v>8</v>
@@ -2244,13 +2248,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B82" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C82" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D82" t="s">
         <v>8</v>
@@ -2258,13 +2262,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B83" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C83" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D83" t="s">
         <v>8</v>
@@ -2272,13 +2276,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B84" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C84" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D84" t="s">
         <v>8</v>
@@ -2286,167 +2290,167 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>164</v>
+      </c>
+      <c r="B85" t="s">
+        <v>205</v>
+      </c>
+      <c r="C85" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85" t="s">
         <v>166</v>
-      </c>
-      <c r="B85" t="s">
-        <v>207</v>
-      </c>
-      <c r="C85" t="s">
-        <v>167</v>
-      </c>
-      <c r="D85" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B86" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C86" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D86" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B87" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C87" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D87" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B88" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C88" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D88" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B89" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C89" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D89" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B90" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C90" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D90" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B91" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C91" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D91" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B92" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C92" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D92" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B93" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C93" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D93" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B94" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C94" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D94" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C95" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D95" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B96" t="s">
         <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>8</v>
@@ -2454,27 +2458,27 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C97" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D97" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C98" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>8</v>
@@ -2482,13 +2486,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C99" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>8</v>
@@ -2496,13 +2500,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B100" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C100" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D100" t="s">
         <v>8</v>
@@ -2510,27 +2514,27 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B101" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C101" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D101" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B102" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C102" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D102" t="s">
         <v>8</v>
@@ -2538,13 +2542,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B103" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C103" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D103" t="s">
         <v>8</v>
@@ -2552,13 +2556,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B104" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C104" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D104" t="s">
         <v>8</v>
@@ -2566,13 +2570,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B105" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C105" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D105" t="s">
         <v>8</v>
@@ -2580,13 +2584,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B106" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C106" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D106" t="s">
         <v>8</v>
@@ -2594,13 +2598,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B107" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C107" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D107" t="s">
         <v>8</v>
@@ -2608,13 +2612,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B108" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C108" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D108" t="s">
         <v>8</v>
@@ -2622,13 +2626,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B109" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C109" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D109" t="s">
         <v>8</v>
@@ -2636,13 +2640,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B110" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C110" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D110" t="s">
         <v>8</v>
@@ -2650,13 +2654,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B111" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C111" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D111" t="s">
         <v>8</v>
@@ -2664,13 +2668,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B112" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C112" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D112" t="s">
         <v>8</v>
@@ -2678,13 +2682,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B113" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C113" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D113" t="s">
         <v>8</v>

</xml_diff>